<commit_message>
update add rating #2
</commit_message>
<xml_diff>
--- a/CFpython/data_recommened_product.xlsx
+++ b/CFpython/data_recommened_product.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -425,10 +425,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1513,45 +1513,23 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B98" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C98" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B99" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C99" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>6</v>
-      </c>
-      <c r="B100" t="n">
-        <v>11</v>
-      </c>
-      <c r="C100" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>20</v>
-      </c>
-      <c r="B101" t="n">
-        <v>5</v>
-      </c>
-      <c r="C101" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update limit product recommend
</commit_message>
<xml_diff>
--- a/CFpython/data_recommened_product.xlsx
+++ b/CFpython/data_recommened_product.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
       <selection activeCell="E106" sqref="E106"/>
@@ -1533,6 +1533,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>15</v>
+      </c>
+      <c r="B100" t="n">
+        <v>4</v>
+      </c>
+      <c r="C100" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>15</v>
+      </c>
+      <c r="B101" t="n">
+        <v>7</v>
+      </c>
+      <c r="C101" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>